<commit_message>
Update stats but needs polishing
</commit_message>
<xml_diff>
--- a/kruskal_tests.xlsx
+++ b/kruskal_tests.xlsx
@@ -34,7 +34,7 @@
       <sz val="9"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -51,6 +51,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00E8E8E8"/>
         <bgColor rgb="00E8E8E8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFA500"/>
+        <bgColor rgb="00FFA500"/>
       </patternFill>
     </fill>
   </fills>
@@ -72,7 +78,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -80,6 +86,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -833,7 +840,7 @@
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>65.916</v>
+        <v>62.934</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>4</v>
@@ -863,7 +870,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>0.655</v>
+        <v>0.624</v>
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
@@ -900,79 +907,87 @@
       <c r="X5" s="2" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>Kruskal-Wallis H test</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>4.073</v>
-      </c>
-      <c r="D6" t="n">
+      <c r="C6" s="2" t="n">
+        <v>10.44</v>
+      </c>
+      <c r="D6" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" s="2" t="inlineStr">
         <is>
           <t>[50, 50, 50]</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" s="2" t="inlineStr">
         <is>
           <t>['Condition A', 'Condition B', 'Condition C']</t>
         </is>
       </c>
-      <c r="G6" s="4" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>ns</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
+      <c r="G6" s="5" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="H6" s="2" t="inlineStr">
+        <is>
+          <t>**</t>
+        </is>
+      </c>
+      <c r="I6" s="2" t="n">
         <v>0.05</v>
       </c>
-      <c r="J6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.014</v>
-      </c>
-      <c r="L6" t="inlineStr">
+      <c r="J6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>0.057</v>
+      </c>
+      <c r="L6" s="2" t="inlineStr">
         <is>
           <t>epsilon-squared</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="M6" s="2" t="inlineStr">
         <is>
           <t>small</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="N6" s="2" t="inlineStr">
         <is>
           <t>All groups have the same population median</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>No significant difference between groups.</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
+      <c r="O6" s="2" t="inlineStr">
+        <is>
+          <t>Significant difference detected. Perform post-hoc pairwise comparisons with test_brunner_munzel() and apply correction (correct_bonferroni or correct_fdr).</t>
+        </is>
+      </c>
+      <c r="P6" s="2" t="inlineStr">
         <is>
           <t>two-sided</t>
         </is>
       </c>
+      <c r="Q6" s="2" t="inlineStr"/>
+      <c r="R6" s="2" t="inlineStr"/>
+      <c r="S6" s="2" t="inlineStr"/>
+      <c r="T6" s="2" t="inlineStr"/>
+      <c r="U6" s="2" t="inlineStr"/>
+      <c r="V6" s="2" t="inlineStr"/>
+      <c r="W6" s="2" t="inlineStr"/>
+      <c r="X6" s="2" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="inlineStr">
-        <is>
-          <t>Generated by SciTeX Stats | 2025-10-01 05:20:40</t>
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>Generated by SciTeX Stats | 2025-10-01 18:14:53</t>
         </is>
       </c>
     </row>

</xml_diff>